<commit_message>
unformatted, added all banks.
</commit_message>
<xml_diff>
--- a/master_BIN.xlsx
+++ b/master_BIN.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1460" uniqueCount="162">
   <si>
     <t>CardName</t>
   </si>
@@ -479,13 +479,34 @@
   </si>
   <si>
     <t xml:space="preserve">MASTER  FLEXI   </t>
+  </si>
+  <si>
+    <t>Finans</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>Kredi kartı</t>
+  </si>
+  <si>
+    <t>Banka kartı</t>
+  </si>
+  <si>
+    <t>Anadolubank</t>
+  </si>
+  <si>
+    <t>Vakıfbank</t>
+  </si>
+  <si>
+    <t>Yapı Kredi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -555,13 +576,26 @@
       <family val="2"/>
       <charset val="162"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -576,7 +610,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -621,6 +655,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -923,10 +960,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H211"/>
+  <dimension ref="A1:H391"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
-      <selection activeCell="D200" sqref="D200"/>
+    <sheetView tabSelected="1" topLeftCell="A254" workbookViewId="0">
+      <selection activeCell="J267" sqref="J267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -934,6 +971,7 @@
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -4783,6 +4821,2526 @@
         <v>548935</v>
       </c>
     </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>155</v>
+      </c>
+      <c r="B212" t="s">
+        <v>155</v>
+      </c>
+      <c r="E212" t="s">
+        <v>41</v>
+      </c>
+      <c r="F212">
+        <v>406386</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>155</v>
+      </c>
+      <c r="B213" t="s">
+        <v>155</v>
+      </c>
+      <c r="E213" t="s">
+        <v>41</v>
+      </c>
+      <c r="F213">
+        <v>415956</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>155</v>
+      </c>
+      <c r="B214" t="s">
+        <v>155</v>
+      </c>
+      <c r="E214" t="s">
+        <v>41</v>
+      </c>
+      <c r="F214">
+        <v>420092</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>155</v>
+      </c>
+      <c r="B215" t="s">
+        <v>155</v>
+      </c>
+      <c r="E215" t="s">
+        <v>41</v>
+      </c>
+      <c r="F215">
+        <v>431379</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>155</v>
+      </c>
+      <c r="B216" t="s">
+        <v>155</v>
+      </c>
+      <c r="E216" t="s">
+        <v>41</v>
+      </c>
+      <c r="F216">
+        <v>459333</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>155</v>
+      </c>
+      <c r="B217" t="s">
+        <v>155</v>
+      </c>
+      <c r="E217" t="s">
+        <v>41</v>
+      </c>
+      <c r="F217">
+        <v>499853</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>155</v>
+      </c>
+      <c r="B218" t="s">
+        <v>155</v>
+      </c>
+      <c r="E218" t="s">
+        <v>41</v>
+      </c>
+      <c r="F218">
+        <v>601050</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>155</v>
+      </c>
+      <c r="B219" t="s">
+        <v>155</v>
+      </c>
+      <c r="E219" t="s">
+        <v>41</v>
+      </c>
+      <c r="F219">
+        <v>677238</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>155</v>
+      </c>
+      <c r="B220" t="s">
+        <v>155</v>
+      </c>
+      <c r="E220" t="s">
+        <v>42</v>
+      </c>
+      <c r="F220">
+        <v>402277</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>155</v>
+      </c>
+      <c r="B221" t="s">
+        <v>155</v>
+      </c>
+      <c r="E221" t="s">
+        <v>42</v>
+      </c>
+      <c r="F221">
+        <v>402278</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>155</v>
+      </c>
+      <c r="B222" t="s">
+        <v>155</v>
+      </c>
+      <c r="E222" t="s">
+        <v>42</v>
+      </c>
+      <c r="F222">
+        <v>402563</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>155</v>
+      </c>
+      <c r="B223" t="s">
+        <v>155</v>
+      </c>
+      <c r="E223" t="s">
+        <v>42</v>
+      </c>
+      <c r="F223">
+        <v>403082</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>155</v>
+      </c>
+      <c r="B224" t="s">
+        <v>155</v>
+      </c>
+      <c r="E224" t="s">
+        <v>42</v>
+      </c>
+      <c r="F224">
+        <v>409364</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>155</v>
+      </c>
+      <c r="B225" t="s">
+        <v>155</v>
+      </c>
+      <c r="E225" t="s">
+        <v>42</v>
+      </c>
+      <c r="F225">
+        <v>410147</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>155</v>
+      </c>
+      <c r="B226" t="s">
+        <v>155</v>
+      </c>
+      <c r="E226" t="s">
+        <v>42</v>
+      </c>
+      <c r="F226">
+        <v>413583</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>155</v>
+      </c>
+      <c r="B227" t="s">
+        <v>155</v>
+      </c>
+      <c r="E227" t="s">
+        <v>42</v>
+      </c>
+      <c r="F227">
+        <v>414388</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>155</v>
+      </c>
+      <c r="B228" t="s">
+        <v>155</v>
+      </c>
+      <c r="E228" t="s">
+        <v>42</v>
+      </c>
+      <c r="F228">
+        <v>415565</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>155</v>
+      </c>
+      <c r="B229" t="s">
+        <v>155</v>
+      </c>
+      <c r="E229" t="s">
+        <v>42</v>
+      </c>
+      <c r="F229">
+        <v>422376</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>155</v>
+      </c>
+      <c r="B230" t="s">
+        <v>155</v>
+      </c>
+      <c r="E230" t="s">
+        <v>42</v>
+      </c>
+      <c r="F230">
+        <v>423277</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>155</v>
+      </c>
+      <c r="B231" t="s">
+        <v>155</v>
+      </c>
+      <c r="E231" t="s">
+        <v>42</v>
+      </c>
+      <c r="F231">
+        <v>423398</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>155</v>
+      </c>
+      <c r="B232" t="s">
+        <v>155</v>
+      </c>
+      <c r="E232" t="s">
+        <v>42</v>
+      </c>
+      <c r="F232">
+        <v>427311</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>155</v>
+      </c>
+      <c r="B233" t="s">
+        <v>155</v>
+      </c>
+      <c r="E233" t="s">
+        <v>42</v>
+      </c>
+      <c r="F233">
+        <v>435653</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>155</v>
+      </c>
+      <c r="B234" t="s">
+        <v>155</v>
+      </c>
+      <c r="E234" t="s">
+        <v>42</v>
+      </c>
+      <c r="F234">
+        <v>441007</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>155</v>
+      </c>
+      <c r="B235" t="s">
+        <v>155</v>
+      </c>
+      <c r="E235" t="s">
+        <v>42</v>
+      </c>
+      <c r="F235">
+        <v>442395</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>155</v>
+      </c>
+      <c r="B236" t="s">
+        <v>155</v>
+      </c>
+      <c r="E236" t="s">
+        <v>42</v>
+      </c>
+      <c r="F236">
+        <v>444029</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>155</v>
+      </c>
+      <c r="B237" t="s">
+        <v>155</v>
+      </c>
+      <c r="E237" t="s">
+        <v>42</v>
+      </c>
+      <c r="F237">
+        <v>459332</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>155</v>
+      </c>
+      <c r="B238" t="s">
+        <v>155</v>
+      </c>
+      <c r="E238" t="s">
+        <v>42</v>
+      </c>
+      <c r="F238">
+        <v>499850</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>155</v>
+      </c>
+      <c r="B239" t="s">
+        <v>155</v>
+      </c>
+      <c r="E239" t="s">
+        <v>42</v>
+      </c>
+      <c r="F239">
+        <v>499851</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>155</v>
+      </c>
+      <c r="B240" t="s">
+        <v>155</v>
+      </c>
+      <c r="E240" t="s">
+        <v>42</v>
+      </c>
+      <c r="F240">
+        <v>499852</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>155</v>
+      </c>
+      <c r="B241" t="s">
+        <v>155</v>
+      </c>
+      <c r="E241" t="s">
+        <v>42</v>
+      </c>
+      <c r="F241">
+        <v>519324</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>155</v>
+      </c>
+      <c r="B242" t="s">
+        <v>155</v>
+      </c>
+      <c r="E242" t="s">
+        <v>42</v>
+      </c>
+      <c r="F242">
+        <v>521022</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>155</v>
+      </c>
+      <c r="B243" t="s">
+        <v>155</v>
+      </c>
+      <c r="E243" t="s">
+        <v>42</v>
+      </c>
+      <c r="F243">
+        <v>521836</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>155</v>
+      </c>
+      <c r="B244" t="s">
+        <v>155</v>
+      </c>
+      <c r="E244" t="s">
+        <v>42</v>
+      </c>
+      <c r="F244">
+        <v>529572</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>155</v>
+      </c>
+      <c r="B245" t="s">
+        <v>155</v>
+      </c>
+      <c r="E245" t="s">
+        <v>42</v>
+      </c>
+      <c r="F245">
+        <v>530818</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>155</v>
+      </c>
+      <c r="B246" t="s">
+        <v>155</v>
+      </c>
+      <c r="E246" t="s">
+        <v>42</v>
+      </c>
+      <c r="F246">
+        <v>531157</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>155</v>
+      </c>
+      <c r="B247" t="s">
+        <v>155</v>
+      </c>
+      <c r="E247" t="s">
+        <v>42</v>
+      </c>
+      <c r="F247">
+        <v>542404</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>155</v>
+      </c>
+      <c r="B248" t="s">
+        <v>155</v>
+      </c>
+      <c r="E248" t="s">
+        <v>42</v>
+      </c>
+      <c r="F248">
+        <v>545120</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>155</v>
+      </c>
+      <c r="B249" t="s">
+        <v>155</v>
+      </c>
+      <c r="E249" t="s">
+        <v>42</v>
+      </c>
+      <c r="F249">
+        <v>545616</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>155</v>
+      </c>
+      <c r="B250" t="s">
+        <v>155</v>
+      </c>
+      <c r="E250" t="s">
+        <v>42</v>
+      </c>
+      <c r="F250">
+        <v>545847</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>155</v>
+      </c>
+      <c r="B251" t="s">
+        <v>155</v>
+      </c>
+      <c r="E251" t="s">
+        <v>42</v>
+      </c>
+      <c r="F251">
+        <v>547567</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>155</v>
+      </c>
+      <c r="B252" t="s">
+        <v>155</v>
+      </c>
+      <c r="E252" t="s">
+        <v>42</v>
+      </c>
+      <c r="F252">
+        <v>547800</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>4</v>
+      </c>
+      <c r="B253" t="s">
+        <v>156</v>
+      </c>
+      <c r="E253" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="F253" s="19">
+        <v>450803</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>4</v>
+      </c>
+      <c r="B254" t="s">
+        <v>156</v>
+      </c>
+      <c r="E254" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="F254" s="19">
+        <v>454360</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>4</v>
+      </c>
+      <c r="B255" t="s">
+        <v>156</v>
+      </c>
+      <c r="E255" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="F255" s="19">
+        <v>454359</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>4</v>
+      </c>
+      <c r="B256" t="s">
+        <v>156</v>
+      </c>
+      <c r="E256" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="F256" s="19">
+        <v>454358</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>4</v>
+      </c>
+      <c r="B257" t="s">
+        <v>156</v>
+      </c>
+      <c r="E257" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="F257" s="19">
+        <v>540667</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>4</v>
+      </c>
+      <c r="B258" t="s">
+        <v>156</v>
+      </c>
+      <c r="E258" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="F258" s="19">
+        <v>540668</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>4</v>
+      </c>
+      <c r="B259" t="s">
+        <v>156</v>
+      </c>
+      <c r="E259" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="F259" s="19">
+        <v>543771</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>4</v>
+      </c>
+      <c r="B260" t="s">
+        <v>156</v>
+      </c>
+      <c r="E260" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="F260" s="19">
+        <v>552096</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>4</v>
+      </c>
+      <c r="B261" t="s">
+        <v>156</v>
+      </c>
+      <c r="E261" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="F261" s="19">
+        <v>510152</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>4</v>
+      </c>
+      <c r="B262" t="s">
+        <v>156</v>
+      </c>
+      <c r="E262" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="F262" s="19">
+        <v>418342</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>4</v>
+      </c>
+      <c r="B263" t="s">
+        <v>156</v>
+      </c>
+      <c r="E263" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="F263" s="19">
+        <v>418343</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>4</v>
+      </c>
+      <c r="B264" t="s">
+        <v>156</v>
+      </c>
+      <c r="E264" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="F264" s="19">
+        <v>418344</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>4</v>
+      </c>
+      <c r="B265" t="s">
+        <v>156</v>
+      </c>
+      <c r="E265" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="F265" s="19">
+        <v>418345</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>4</v>
+      </c>
+      <c r="B266" t="s">
+        <v>156</v>
+      </c>
+      <c r="E266" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="F266" s="19">
+        <v>414314</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>4</v>
+      </c>
+      <c r="B267" t="s">
+        <v>156</v>
+      </c>
+      <c r="E267" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="F267" s="19">
+        <v>589283</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>4</v>
+      </c>
+      <c r="B268" t="s">
+        <v>156</v>
+      </c>
+      <c r="E268" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="F268">
+        <v>444676</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>4</v>
+      </c>
+      <c r="B269" t="s">
+        <v>156</v>
+      </c>
+      <c r="E269" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="F269">
+        <v>444677</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>4</v>
+      </c>
+      <c r="B270" t="s">
+        <v>156</v>
+      </c>
+      <c r="E270" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="F270">
+        <v>444678</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>4</v>
+      </c>
+      <c r="B271" t="s">
+        <v>156</v>
+      </c>
+      <c r="E271" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="F271">
+        <v>534981</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>4</v>
+      </c>
+      <c r="B272" t="s">
+        <v>156</v>
+      </c>
+      <c r="E272" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="F272">
+        <v>469894</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>4</v>
+      </c>
+      <c r="B273" t="s">
+        <v>156</v>
+      </c>
+      <c r="E273" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="F273">
+        <v>542374</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>4</v>
+      </c>
+      <c r="B274" t="s">
+        <v>156</v>
+      </c>
+      <c r="E274" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="F274">
+        <v>454314</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>4</v>
+      </c>
+      <c r="B275" t="s">
+        <v>156</v>
+      </c>
+      <c r="E275" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="F275">
+        <v>589283</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>161</v>
+      </c>
+      <c r="B276" t="s">
+        <v>159</v>
+      </c>
+      <c r="E276" t="s">
+        <v>42</v>
+      </c>
+      <c r="F276">
+        <v>425846</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>161</v>
+      </c>
+      <c r="B277" t="s">
+        <v>159</v>
+      </c>
+      <c r="E277" t="s">
+        <v>42</v>
+      </c>
+      <c r="F277">
+        <v>425847</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>161</v>
+      </c>
+      <c r="B278" t="s">
+        <v>159</v>
+      </c>
+      <c r="E278" t="s">
+        <v>42</v>
+      </c>
+      <c r="F278">
+        <v>425848</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>161</v>
+      </c>
+      <c r="B279" t="s">
+        <v>159</v>
+      </c>
+      <c r="E279" t="s">
+        <v>42</v>
+      </c>
+      <c r="F279">
+        <v>425849</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>161</v>
+      </c>
+      <c r="B280" t="s">
+        <v>159</v>
+      </c>
+      <c r="E280" t="s">
+        <v>42</v>
+      </c>
+      <c r="F280">
+        <v>441341</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>161</v>
+      </c>
+      <c r="B281" t="s">
+        <v>159</v>
+      </c>
+      <c r="E281" t="s">
+        <v>42</v>
+      </c>
+      <c r="F281">
+        <v>522240</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>161</v>
+      </c>
+      <c r="B282" t="s">
+        <v>159</v>
+      </c>
+      <c r="E282" t="s">
+        <v>42</v>
+      </c>
+      <c r="F282">
+        <v>522241</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>161</v>
+      </c>
+      <c r="B283" t="s">
+        <v>159</v>
+      </c>
+      <c r="E283" t="s">
+        <v>42</v>
+      </c>
+      <c r="F283">
+        <v>554301</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>161</v>
+      </c>
+      <c r="B284" t="s">
+        <v>159</v>
+      </c>
+      <c r="E284" t="s">
+        <v>42</v>
+      </c>
+      <c r="F284">
+        <v>558593</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>161</v>
+      </c>
+      <c r="B285" t="s">
+        <v>159</v>
+      </c>
+      <c r="E285" t="s">
+        <v>41</v>
+      </c>
+      <c r="F285">
+        <v>676460</v>
+      </c>
+    </row>
+    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>161</v>
+      </c>
+      <c r="B286" t="s">
+        <v>160</v>
+      </c>
+      <c r="E286" t="s">
+        <v>42</v>
+      </c>
+      <c r="F286">
+        <v>402940</v>
+      </c>
+    </row>
+    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>161</v>
+      </c>
+      <c r="B287" t="s">
+        <v>160</v>
+      </c>
+      <c r="E287" t="s">
+        <v>42</v>
+      </c>
+      <c r="F287">
+        <v>409084</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>161</v>
+      </c>
+      <c r="B288" t="s">
+        <v>160</v>
+      </c>
+      <c r="E288" t="s">
+        <v>42</v>
+      </c>
+      <c r="F288">
+        <v>411724</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>161</v>
+      </c>
+      <c r="B289" t="s">
+        <v>160</v>
+      </c>
+      <c r="E289" t="s">
+        <v>42</v>
+      </c>
+      <c r="F289">
+        <v>411942</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>161</v>
+      </c>
+      <c r="B290" t="s">
+        <v>160</v>
+      </c>
+      <c r="E290" t="s">
+        <v>42</v>
+      </c>
+      <c r="F290">
+        <v>411943</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>161</v>
+      </c>
+      <c r="B291" t="s">
+        <v>160</v>
+      </c>
+      <c r="E291" t="s">
+        <v>42</v>
+      </c>
+      <c r="F291">
+        <v>411944</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>161</v>
+      </c>
+      <c r="B292" t="s">
+        <v>160</v>
+      </c>
+      <c r="E292" t="s">
+        <v>42</v>
+      </c>
+      <c r="F292">
+        <v>411979</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>161</v>
+      </c>
+      <c r="B293" t="s">
+        <v>160</v>
+      </c>
+      <c r="E293" t="s">
+        <v>42</v>
+      </c>
+      <c r="F293">
+        <v>415792</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>161</v>
+      </c>
+      <c r="B294" t="s">
+        <v>160</v>
+      </c>
+      <c r="E294" t="s">
+        <v>42</v>
+      </c>
+      <c r="F294">
+        <v>416757</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>161</v>
+      </c>
+      <c r="B295" t="s">
+        <v>160</v>
+      </c>
+      <c r="E295" t="s">
+        <v>42</v>
+      </c>
+      <c r="F295">
+        <v>428945</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>161</v>
+      </c>
+      <c r="B296" t="s">
+        <v>160</v>
+      </c>
+      <c r="E296" t="s">
+        <v>42</v>
+      </c>
+      <c r="F296">
+        <v>442671</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>161</v>
+      </c>
+      <c r="B297" t="s">
+        <v>160</v>
+      </c>
+      <c r="E297" t="s">
+        <v>41</v>
+      </c>
+      <c r="F297">
+        <v>491005</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>161</v>
+      </c>
+      <c r="B298" t="s">
+        <v>160</v>
+      </c>
+      <c r="E298" t="s">
+        <v>42</v>
+      </c>
+      <c r="F298">
+        <v>493840</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>161</v>
+      </c>
+      <c r="B299" t="s">
+        <v>160</v>
+      </c>
+      <c r="E299" t="s">
+        <v>42</v>
+      </c>
+      <c r="F299">
+        <v>493841</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
+        <v>161</v>
+      </c>
+      <c r="B300" t="s">
+        <v>160</v>
+      </c>
+      <c r="E300" t="s">
+        <v>42</v>
+      </c>
+      <c r="F300">
+        <v>493846</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>161</v>
+      </c>
+      <c r="B301" t="s">
+        <v>160</v>
+      </c>
+      <c r="E301" t="s">
+        <v>42</v>
+      </c>
+      <c r="F301">
+        <v>510162</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>161</v>
+      </c>
+      <c r="B302" t="s">
+        <v>160</v>
+      </c>
+      <c r="E302" t="s">
+        <v>42</v>
+      </c>
+      <c r="F302">
+        <v>510163</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>161</v>
+      </c>
+      <c r="B303" t="s">
+        <v>160</v>
+      </c>
+      <c r="E303" t="s">
+        <v>42</v>
+      </c>
+      <c r="F303">
+        <v>510238</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
+        <v>161</v>
+      </c>
+      <c r="B304" t="s">
+        <v>160</v>
+      </c>
+      <c r="E304" t="s">
+        <v>42</v>
+      </c>
+      <c r="F304">
+        <v>520017</v>
+      </c>
+    </row>
+    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>161</v>
+      </c>
+      <c r="B305" t="s">
+        <v>160</v>
+      </c>
+      <c r="E305" t="s">
+        <v>42</v>
+      </c>
+      <c r="F305">
+        <v>540045</v>
+      </c>
+    </row>
+    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
+        <v>161</v>
+      </c>
+      <c r="B306" t="s">
+        <v>160</v>
+      </c>
+      <c r="E306" t="s">
+        <v>42</v>
+      </c>
+      <c r="F306">
+        <v>540046</v>
+      </c>
+    </row>
+    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>161</v>
+      </c>
+      <c r="B307" t="s">
+        <v>160</v>
+      </c>
+      <c r="E307" t="s">
+        <v>42</v>
+      </c>
+      <c r="F307">
+        <v>542119</v>
+      </c>
+    </row>
+    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
+        <v>161</v>
+      </c>
+      <c r="B308" t="s">
+        <v>160</v>
+      </c>
+      <c r="E308" t="s">
+        <v>42</v>
+      </c>
+      <c r="F308">
+        <v>542798</v>
+      </c>
+    </row>
+    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
+        <v>161</v>
+      </c>
+      <c r="B309" t="s">
+        <v>160</v>
+      </c>
+      <c r="E309" t="s">
+        <v>42</v>
+      </c>
+      <c r="F309">
+        <v>542804</v>
+      </c>
+    </row>
+    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
+        <v>161</v>
+      </c>
+      <c r="B310" t="s">
+        <v>160</v>
+      </c>
+      <c r="E310" t="s">
+        <v>42</v>
+      </c>
+      <c r="F310">
+        <v>547244</v>
+      </c>
+    </row>
+    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
+        <v>161</v>
+      </c>
+      <c r="B311" t="s">
+        <v>160</v>
+      </c>
+      <c r="E311" t="s">
+        <v>42</v>
+      </c>
+      <c r="F311">
+        <v>552101</v>
+      </c>
+    </row>
+    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
+        <v>161</v>
+      </c>
+      <c r="B312" t="s">
+        <v>160</v>
+      </c>
+      <c r="E312" t="s">
+        <v>41</v>
+      </c>
+      <c r="F312">
+        <v>589311</v>
+      </c>
+    </row>
+    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
+        <v>161</v>
+      </c>
+      <c r="B313" t="s">
+        <v>160</v>
+      </c>
+      <c r="E313" t="s">
+        <v>41</v>
+      </c>
+      <c r="F313">
+        <v>990015</v>
+      </c>
+    </row>
+    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
+        <v>161</v>
+      </c>
+      <c r="B314" t="s">
+        <v>107</v>
+      </c>
+      <c r="E314" t="s">
+        <v>42</v>
+      </c>
+      <c r="F314">
+        <v>402458</v>
+      </c>
+    </row>
+    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A315" t="s">
+        <v>161</v>
+      </c>
+      <c r="B315" t="s">
+        <v>107</v>
+      </c>
+      <c r="E315" t="s">
+        <v>42</v>
+      </c>
+      <c r="F315">
+        <v>402459</v>
+      </c>
+    </row>
+    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A316" t="s">
+        <v>161</v>
+      </c>
+      <c r="B316" t="s">
+        <v>107</v>
+      </c>
+      <c r="E316" t="s">
+        <v>42</v>
+      </c>
+      <c r="F316">
+        <v>406015</v>
+      </c>
+    </row>
+    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A317" t="s">
+        <v>161</v>
+      </c>
+      <c r="B317" t="s">
+        <v>107</v>
+      </c>
+      <c r="E317" t="s">
+        <v>42</v>
+      </c>
+      <c r="F317">
+        <v>427707</v>
+      </c>
+    </row>
+    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A318" t="s">
+        <v>161</v>
+      </c>
+      <c r="B318" t="s">
+        <v>107</v>
+      </c>
+      <c r="E318" t="s">
+        <v>42</v>
+      </c>
+      <c r="F318">
+        <v>440247</v>
+      </c>
+    </row>
+    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A319" t="s">
+        <v>161</v>
+      </c>
+      <c r="B319" t="s">
+        <v>107</v>
+      </c>
+      <c r="E319" t="s">
+        <v>42</v>
+      </c>
+      <c r="F319">
+        <v>440273</v>
+      </c>
+    </row>
+    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
+        <v>161</v>
+      </c>
+      <c r="B320" t="s">
+        <v>107</v>
+      </c>
+      <c r="E320" t="s">
+        <v>41</v>
+      </c>
+      <c r="F320">
+        <v>440274</v>
+      </c>
+    </row>
+    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>161</v>
+      </c>
+      <c r="B321" t="s">
+        <v>107</v>
+      </c>
+      <c r="E321" t="s">
+        <v>42</v>
+      </c>
+      <c r="F321">
+        <v>440293</v>
+      </c>
+    </row>
+    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A322" t="s">
+        <v>161</v>
+      </c>
+      <c r="B322" t="s">
+        <v>107</v>
+      </c>
+      <c r="E322" t="s">
+        <v>42</v>
+      </c>
+      <c r="F322">
+        <v>440294</v>
+      </c>
+    </row>
+    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A323" t="s">
+        <v>161</v>
+      </c>
+      <c r="B323" t="s">
+        <v>107</v>
+      </c>
+      <c r="E323" t="s">
+        <v>42</v>
+      </c>
+      <c r="F323">
+        <v>440295</v>
+      </c>
+    </row>
+    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A324" t="s">
+        <v>161</v>
+      </c>
+      <c r="B324" t="s">
+        <v>107</v>
+      </c>
+      <c r="E324" t="s">
+        <v>42</v>
+      </c>
+      <c r="F324">
+        <v>459026</v>
+      </c>
+    </row>
+    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
+        <v>161</v>
+      </c>
+      <c r="B325" t="s">
+        <v>107</v>
+      </c>
+      <c r="E325" t="s">
+        <v>42</v>
+      </c>
+      <c r="F325">
+        <v>479227</v>
+      </c>
+    </row>
+    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>161</v>
+      </c>
+      <c r="B326" t="s">
+        <v>107</v>
+      </c>
+      <c r="E326" t="s">
+        <v>42</v>
+      </c>
+      <c r="F326">
+        <v>489494</v>
+      </c>
+    </row>
+    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
+        <v>161</v>
+      </c>
+      <c r="B327" t="s">
+        <v>107</v>
+      </c>
+      <c r="E327" t="s">
+        <v>42</v>
+      </c>
+      <c r="F327">
+        <v>489495</v>
+      </c>
+    </row>
+    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
+        <v>161</v>
+      </c>
+      <c r="B328" t="s">
+        <v>107</v>
+      </c>
+      <c r="E328" t="s">
+        <v>42</v>
+      </c>
+      <c r="F328">
+        <v>489496</v>
+      </c>
+    </row>
+    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
+        <v>161</v>
+      </c>
+      <c r="B329" t="s">
+        <v>107</v>
+      </c>
+      <c r="E329" t="s">
+        <v>42</v>
+      </c>
+      <c r="F329">
+        <v>510138</v>
+      </c>
+    </row>
+    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A330" t="s">
+        <v>161</v>
+      </c>
+      <c r="B330" t="s">
+        <v>107</v>
+      </c>
+      <c r="E330" t="s">
+        <v>42</v>
+      </c>
+      <c r="F330">
+        <v>510139</v>
+      </c>
+    </row>
+    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A331" t="s">
+        <v>161</v>
+      </c>
+      <c r="B331" t="s">
+        <v>107</v>
+      </c>
+      <c r="E331" t="s">
+        <v>42</v>
+      </c>
+      <c r="F331">
+        <v>510221</v>
+      </c>
+    </row>
+    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
+        <v>161</v>
+      </c>
+      <c r="B332" t="s">
+        <v>107</v>
+      </c>
+      <c r="E332" t="s">
+        <v>42</v>
+      </c>
+      <c r="F332">
+        <v>512753</v>
+      </c>
+    </row>
+    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A333" t="s">
+        <v>161</v>
+      </c>
+      <c r="B333" t="s">
+        <v>107</v>
+      </c>
+      <c r="E333" t="s">
+        <v>42</v>
+      </c>
+      <c r="F333">
+        <v>512803</v>
+      </c>
+    </row>
+    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A334" t="s">
+        <v>161</v>
+      </c>
+      <c r="B334" t="s">
+        <v>107</v>
+      </c>
+      <c r="E334" t="s">
+        <v>41</v>
+      </c>
+      <c r="F334">
+        <v>516742</v>
+      </c>
+    </row>
+    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A335" t="s">
+        <v>161</v>
+      </c>
+      <c r="B335" t="s">
+        <v>107</v>
+      </c>
+      <c r="E335" t="s">
+        <v>42</v>
+      </c>
+      <c r="F335">
+        <v>524346</v>
+      </c>
+    </row>
+    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A336" t="s">
+        <v>161</v>
+      </c>
+      <c r="B336" t="s">
+        <v>107</v>
+      </c>
+      <c r="E336" t="s">
+        <v>42</v>
+      </c>
+      <c r="F336">
+        <v>524839</v>
+      </c>
+    </row>
+    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
+        <v>161</v>
+      </c>
+      <c r="B337" t="s">
+        <v>107</v>
+      </c>
+      <c r="E337" t="s">
+        <v>42</v>
+      </c>
+      <c r="F337">
+        <v>524840</v>
+      </c>
+    </row>
+    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A338" t="s">
+        <v>161</v>
+      </c>
+      <c r="B338" t="s">
+        <v>107</v>
+      </c>
+      <c r="E338" t="s">
+        <v>42</v>
+      </c>
+      <c r="F338">
+        <v>528920</v>
+      </c>
+    </row>
+    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A339" t="s">
+        <v>161</v>
+      </c>
+      <c r="B339" t="s">
+        <v>107</v>
+      </c>
+      <c r="E339" t="s">
+        <v>42</v>
+      </c>
+      <c r="F339">
+        <v>530853</v>
+      </c>
+    </row>
+    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A340" t="s">
+        <v>161</v>
+      </c>
+      <c r="B340" t="s">
+        <v>107</v>
+      </c>
+      <c r="E340" t="s">
+        <v>42</v>
+      </c>
+      <c r="F340">
+        <v>545124</v>
+      </c>
+    </row>
+    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A341" t="s">
+        <v>161</v>
+      </c>
+      <c r="B341" t="s">
+        <v>107</v>
+      </c>
+      <c r="E341" t="s">
+        <v>42</v>
+      </c>
+      <c r="F341">
+        <v>553090</v>
+      </c>
+    </row>
+    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A342" t="s">
+        <v>161</v>
+      </c>
+      <c r="B342" t="s">
+        <v>107</v>
+      </c>
+      <c r="E342" t="s">
+        <v>41</v>
+      </c>
+      <c r="F342">
+        <v>676578</v>
+      </c>
+    </row>
+    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A343" t="s">
+        <v>161</v>
+      </c>
+      <c r="B343" t="s">
+        <v>161</v>
+      </c>
+      <c r="E343" t="s">
+        <v>41</v>
+      </c>
+      <c r="F343">
+        <v>401622</v>
+      </c>
+    </row>
+    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
+        <v>161</v>
+      </c>
+      <c r="B344" t="s">
+        <v>161</v>
+      </c>
+      <c r="E344" t="s">
+        <v>42</v>
+      </c>
+      <c r="F344">
+        <v>404809</v>
+      </c>
+    </row>
+    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A345" t="s">
+        <v>161</v>
+      </c>
+      <c r="B345" t="s">
+        <v>161</v>
+      </c>
+      <c r="E345" t="s">
+        <v>41</v>
+      </c>
+      <c r="F345">
+        <v>406281</v>
+      </c>
+    </row>
+    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
+        <v>161</v>
+      </c>
+      <c r="B346" t="s">
+        <v>161</v>
+      </c>
+      <c r="E346" t="s">
+        <v>42</v>
+      </c>
+      <c r="F346">
+        <v>408522</v>
+      </c>
+    </row>
+    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
+        <v>161</v>
+      </c>
+      <c r="B347" t="s">
+        <v>161</v>
+      </c>
+      <c r="E347" t="s">
+        <v>41</v>
+      </c>
+      <c r="F347">
+        <v>413382</v>
+      </c>
+    </row>
+    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A348" t="s">
+        <v>161</v>
+      </c>
+      <c r="B348" t="s">
+        <v>161</v>
+      </c>
+      <c r="E348" t="s">
+        <v>41</v>
+      </c>
+      <c r="F348">
+        <v>414392</v>
+      </c>
+    </row>
+    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A349" t="s">
+        <v>161</v>
+      </c>
+      <c r="B349" t="s">
+        <v>161</v>
+      </c>
+      <c r="E349" t="s">
+        <v>41</v>
+      </c>
+      <c r="F349">
+        <v>420343</v>
+      </c>
+    </row>
+    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A350" t="s">
+        <v>161</v>
+      </c>
+      <c r="B350" t="s">
+        <v>161</v>
+      </c>
+      <c r="E350" t="s">
+        <v>41</v>
+      </c>
+      <c r="F350">
+        <v>442106</v>
+      </c>
+    </row>
+    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A351" t="s">
+        <v>161</v>
+      </c>
+      <c r="B351" t="s">
+        <v>161</v>
+      </c>
+      <c r="E351" t="s">
+        <v>42</v>
+      </c>
+      <c r="F351">
+        <v>444444</v>
+      </c>
+    </row>
+    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
+        <v>161</v>
+      </c>
+      <c r="B352" t="s">
+        <v>161</v>
+      </c>
+      <c r="E352" t="s">
+        <v>42</v>
+      </c>
+      <c r="F352">
+        <v>446212</v>
+      </c>
+    </row>
+    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
+        <v>161</v>
+      </c>
+      <c r="B353" t="s">
+        <v>161</v>
+      </c>
+      <c r="E353" t="s">
+        <v>42</v>
+      </c>
+      <c r="F353">
+        <v>450634</v>
+      </c>
+    </row>
+    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A354" t="s">
+        <v>161</v>
+      </c>
+      <c r="B354" t="s">
+        <v>161</v>
+      </c>
+      <c r="E354" t="s">
+        <v>42</v>
+      </c>
+      <c r="F354">
+        <v>455359</v>
+      </c>
+    </row>
+    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A355" t="s">
+        <v>161</v>
+      </c>
+      <c r="B355" t="s">
+        <v>161</v>
+      </c>
+      <c r="E355" t="s">
+        <v>42</v>
+      </c>
+      <c r="F355">
+        <v>455360</v>
+      </c>
+    </row>
+    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A356" t="s">
+        <v>161</v>
+      </c>
+      <c r="B356" t="s">
+        <v>161</v>
+      </c>
+      <c r="E356" t="s">
+        <v>42</v>
+      </c>
+      <c r="F356">
+        <v>479794</v>
+      </c>
+    </row>
+    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A357" t="s">
+        <v>161</v>
+      </c>
+      <c r="B357" t="s">
+        <v>161</v>
+      </c>
+      <c r="E357" t="s">
+        <v>42</v>
+      </c>
+      <c r="F357">
+        <v>479795</v>
+      </c>
+    </row>
+    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A358" t="s">
+        <v>161</v>
+      </c>
+      <c r="B358" t="s">
+        <v>161</v>
+      </c>
+      <c r="E358" t="s">
+        <v>41</v>
+      </c>
+      <c r="F358">
+        <v>490983</v>
+      </c>
+    </row>
+    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A359" t="s">
+        <v>161</v>
+      </c>
+      <c r="B359" t="s">
+        <v>161</v>
+      </c>
+      <c r="E359" t="s">
+        <v>42</v>
+      </c>
+      <c r="F359">
+        <v>491205</v>
+      </c>
+    </row>
+    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A360" t="s">
+        <v>161</v>
+      </c>
+      <c r="B360" t="s">
+        <v>161</v>
+      </c>
+      <c r="E360" t="s">
+        <v>42</v>
+      </c>
+      <c r="F360">
+        <v>492129</v>
+      </c>
+    </row>
+    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A361" t="s">
+        <v>161</v>
+      </c>
+      <c r="B361" t="s">
+        <v>161</v>
+      </c>
+      <c r="E361" t="s">
+        <v>42</v>
+      </c>
+      <c r="F361">
+        <v>492130</v>
+      </c>
+    </row>
+    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A362" t="s">
+        <v>161</v>
+      </c>
+      <c r="B362" t="s">
+        <v>161</v>
+      </c>
+      <c r="E362" t="s">
+        <v>42</v>
+      </c>
+      <c r="F362">
+        <v>492131</v>
+      </c>
+    </row>
+    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A363" t="s">
+        <v>161</v>
+      </c>
+      <c r="B363" t="s">
+        <v>161</v>
+      </c>
+      <c r="E363" t="s">
+        <v>41</v>
+      </c>
+      <c r="F363">
+        <v>494314</v>
+      </c>
+    </row>
+    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A364" t="s">
+        <v>161</v>
+      </c>
+      <c r="B364" t="s">
+        <v>161</v>
+      </c>
+      <c r="E364" t="s">
+        <v>41</v>
+      </c>
+      <c r="F364">
+        <v>501774</v>
+      </c>
+    </row>
+    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A365" t="s">
+        <v>161</v>
+      </c>
+      <c r="B365" t="s">
+        <v>161</v>
+      </c>
+      <c r="E365" t="s">
+        <v>42</v>
+      </c>
+      <c r="F365">
+        <v>510054</v>
+      </c>
+    </row>
+    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A366" t="s">
+        <v>161</v>
+      </c>
+      <c r="B366" t="s">
+        <v>161</v>
+      </c>
+      <c r="E366" t="s">
+        <v>42</v>
+      </c>
+      <c r="F366">
+        <v>540061</v>
+      </c>
+    </row>
+    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A367" t="s">
+        <v>161</v>
+      </c>
+      <c r="B367" t="s">
+        <v>161</v>
+      </c>
+      <c r="E367" t="s">
+        <v>42</v>
+      </c>
+      <c r="F367">
+        <v>540062</v>
+      </c>
+    </row>
+    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A368" t="s">
+        <v>161</v>
+      </c>
+      <c r="B368" t="s">
+        <v>161</v>
+      </c>
+      <c r="E368" t="s">
+        <v>42</v>
+      </c>
+      <c r="F368">
+        <v>540063</v>
+      </c>
+    </row>
+    <row r="369" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A369" t="s">
+        <v>161</v>
+      </c>
+      <c r="B369" t="s">
+        <v>161</v>
+      </c>
+      <c r="E369" t="s">
+        <v>42</v>
+      </c>
+      <c r="F369">
+        <v>540122</v>
+      </c>
+    </row>
+    <row r="370" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A370" t="s">
+        <v>161</v>
+      </c>
+      <c r="B370" t="s">
+        <v>161</v>
+      </c>
+      <c r="E370" t="s">
+        <v>42</v>
+      </c>
+      <c r="F370">
+        <v>540129</v>
+      </c>
+    </row>
+    <row r="371" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A371" t="s">
+        <v>161</v>
+      </c>
+      <c r="B371" t="s">
+        <v>161</v>
+      </c>
+      <c r="E371" t="s">
+        <v>42</v>
+      </c>
+      <c r="F371">
+        <v>542117</v>
+      </c>
+    </row>
+    <row r="372" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A372" t="s">
+        <v>161</v>
+      </c>
+      <c r="B372" t="s">
+        <v>161</v>
+      </c>
+      <c r="E372" t="s">
+        <v>42</v>
+      </c>
+      <c r="F372">
+        <v>545103</v>
+      </c>
+    </row>
+    <row r="373" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A373" t="s">
+        <v>161</v>
+      </c>
+      <c r="B373" t="s">
+        <v>161</v>
+      </c>
+      <c r="E373" t="s">
+        <v>42</v>
+      </c>
+      <c r="F373">
+        <v>550054</v>
+      </c>
+    </row>
+    <row r="374" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A374" t="s">
+        <v>161</v>
+      </c>
+      <c r="B374" t="s">
+        <v>161</v>
+      </c>
+      <c r="E374" t="s">
+        <v>42</v>
+      </c>
+      <c r="F374">
+        <v>552645</v>
+      </c>
+    </row>
+    <row r="375" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A375" t="s">
+        <v>161</v>
+      </c>
+      <c r="B375" t="s">
+        <v>161</v>
+      </c>
+      <c r="E375" t="s">
+        <v>42</v>
+      </c>
+      <c r="F375">
+        <v>552659</v>
+      </c>
+    </row>
+    <row r="376" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A376" t="s">
+        <v>161</v>
+      </c>
+      <c r="B376" t="s">
+        <v>161</v>
+      </c>
+      <c r="E376" t="s">
+        <v>41</v>
+      </c>
+      <c r="F376">
+        <v>560279</v>
+      </c>
+    </row>
+    <row r="377" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A377" t="s">
+        <v>161</v>
+      </c>
+      <c r="B377" t="s">
+        <v>161</v>
+      </c>
+      <c r="E377" t="s">
+        <v>41</v>
+      </c>
+      <c r="F377">
+        <v>561056</v>
+      </c>
+    </row>
+    <row r="378" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A378" t="s">
+        <v>161</v>
+      </c>
+      <c r="B378" t="s">
+        <v>161</v>
+      </c>
+      <c r="E378" t="s">
+        <v>41</v>
+      </c>
+      <c r="F378">
+        <v>588691</v>
+      </c>
+    </row>
+    <row r="379" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A379" t="s">
+        <v>161</v>
+      </c>
+      <c r="B379" t="s">
+        <v>161</v>
+      </c>
+      <c r="E379" t="s">
+        <v>41</v>
+      </c>
+      <c r="F379">
+        <v>588992</v>
+      </c>
+    </row>
+    <row r="380" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A380" t="s">
+        <v>161</v>
+      </c>
+      <c r="B380" t="s">
+        <v>161</v>
+      </c>
+      <c r="E380" t="s">
+        <v>41</v>
+      </c>
+      <c r="F380">
+        <v>589117</v>
+      </c>
+    </row>
+    <row r="381" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A381" t="s">
+        <v>161</v>
+      </c>
+      <c r="B381" t="s">
+        <v>161</v>
+      </c>
+      <c r="E381" t="s">
+        <v>42</v>
+      </c>
+      <c r="F381">
+        <v>601881</v>
+      </c>
+    </row>
+    <row r="382" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A382" t="s">
+        <v>161</v>
+      </c>
+      <c r="B382" t="s">
+        <v>161</v>
+      </c>
+      <c r="E382" t="s">
+        <v>42</v>
+      </c>
+      <c r="F382">
+        <v>602676</v>
+      </c>
+    </row>
+    <row r="383" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A383" t="s">
+        <v>161</v>
+      </c>
+      <c r="B383" t="s">
+        <v>161</v>
+      </c>
+      <c r="E383" t="s">
+        <v>42</v>
+      </c>
+      <c r="F383">
+        <v>602678</v>
+      </c>
+    </row>
+    <row r="384" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A384" t="s">
+        <v>161</v>
+      </c>
+      <c r="B384" t="s">
+        <v>161</v>
+      </c>
+      <c r="E384" t="s">
+        <v>42</v>
+      </c>
+      <c r="F384">
+        <v>602908</v>
+      </c>
+    </row>
+    <row r="385" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A385" t="s">
+        <v>161</v>
+      </c>
+      <c r="B385" t="s">
+        <v>161</v>
+      </c>
+      <c r="E385" t="s">
+        <v>42</v>
+      </c>
+      <c r="F385">
+        <v>602981</v>
+      </c>
+    </row>
+    <row r="386" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A386" t="s">
+        <v>161</v>
+      </c>
+      <c r="B386" t="s">
+        <v>161</v>
+      </c>
+      <c r="E386" t="s">
+        <v>42</v>
+      </c>
+      <c r="F386">
+        <v>603098</v>
+      </c>
+    </row>
+    <row r="387" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A387" t="s">
+        <v>161</v>
+      </c>
+      <c r="B387" t="s">
+        <v>161</v>
+      </c>
+      <c r="E387" t="s">
+        <v>41</v>
+      </c>
+      <c r="F387">
+        <v>603649</v>
+      </c>
+    </row>
+    <row r="388" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A388" t="s">
+        <v>161</v>
+      </c>
+      <c r="B388" t="s">
+        <v>161</v>
+      </c>
+      <c r="E388" t="s">
+        <v>41</v>
+      </c>
+      <c r="F388">
+        <v>603797</v>
+      </c>
+    </row>
+    <row r="389" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A389" t="s">
+        <v>161</v>
+      </c>
+      <c r="B389" t="s">
+        <v>161</v>
+      </c>
+      <c r="E389" t="s">
+        <v>41</v>
+      </c>
+      <c r="F389">
+        <v>636689</v>
+      </c>
+    </row>
+    <row r="390" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A390" t="s">
+        <v>161</v>
+      </c>
+      <c r="B390" t="s">
+        <v>161</v>
+      </c>
+      <c r="E390" t="s">
+        <v>41</v>
+      </c>
+      <c r="F390">
+        <v>639004</v>
+      </c>
+    </row>
+    <row r="391" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A391" t="s">
+        <v>161</v>
+      </c>
+      <c r="B391" t="s">
+        <v>161</v>
+      </c>
+      <c r="E391" t="s">
+        <v>41</v>
+      </c>
+      <c r="F391">
+        <v>676166</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>